<commit_message>
loginLogout page is added
</commit_message>
<xml_diff>
--- a/src/test/test_data/prodajaguma.xlsx
+++ b/src/test/test_data/prodajaguma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QAprojekti\Automation_projekti\Internet_ProdajaGuma\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4337DDFB-43FE-44BF-BCD0-329B3A7BD706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C32961-16B4-47C7-BBC8-569B3A4C94EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="automobili" sheetId="1" r:id="rId1"/>
@@ -31,14 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="106">
   <si>
     <t>tc_id</t>
   </si>
   <si>
-    <t>Test import data for "Sindri" project</t>
-  </si>
-  <si>
     <t>SI_001</t>
   </si>
   <si>
@@ -60,21 +57,12 @@
     <t>SI_005</t>
   </si>
   <si>
-    <t>value</t>
-  </si>
-  <si>
     <t>SI_006</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>randomTypeYesNo</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>SI_007</t>
   </si>
   <si>
@@ -87,30 +75,12 @@
     <t>accountRegistered</t>
   </si>
   <si>
-    <t>Thank you for registering with Fake Online Clothing Store.</t>
-  </si>
-  <si>
     <t>invalidMessageCreateAccount</t>
   </si>
   <si>
-    <t>This is a required field.</t>
-  </si>
-  <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>lastname</t>
-  </si>
-  <si>
     <t>SI_009</t>
   </si>
   <si>
-    <t>confirmpassword</t>
-  </si>
-  <si>
-    <t>Please enter a valid email address (Ex: johndoe@domain.com).</t>
-  </si>
-  <si>
     <t>SI_010</t>
   </si>
   <si>
@@ -129,51 +99,12 @@
     <t>SI_015</t>
   </si>
   <si>
-    <t>Password Strength: No Password</t>
-  </si>
-  <si>
-    <t>Password Strength: Weak</t>
-  </si>
-  <si>
-    <t>Password Strength: Very Strong</t>
-  </si>
-  <si>
-    <t>strengthpassword</t>
-  </si>
-  <si>
-    <t>Password Strength: Medium</t>
-  </si>
-  <si>
-    <t>Please enter the same value again.</t>
-  </si>
-  <si>
-    <t>both</t>
-  </si>
-  <si>
-    <t>The account sign-in was incorrect or your account is disabled temporarily. Please wait and try again later.</t>
-  </si>
-  <si>
     <t>invalidMessageCreateAccount2</t>
   </si>
   <si>
-    <t>Incorrect CAPTCHA</t>
-  </si>
-  <si>
     <t>emptyCartMessage</t>
   </si>
   <si>
-    <t>You have no items in your shopping cart.</t>
-  </si>
-  <si>
-    <t>Men</t>
-  </si>
-  <si>
-    <t>Gear</t>
-  </si>
-  <si>
-    <t>Training</t>
-  </si>
-  <si>
     <t>menuItemTitle1</t>
   </si>
   <si>
@@ -183,33 +114,9 @@
     <t>menuItemTitle2</t>
   </si>
   <si>
-    <t>TOPS</t>
-  </si>
-  <si>
-    <t>BOTTOMS</t>
-  </si>
-  <si>
     <t>product</t>
   </si>
   <si>
-    <t>Hoodies &amp; Sweatshirts</t>
-  </si>
-  <si>
-    <t>Jackets</t>
-  </si>
-  <si>
-    <t>Tees</t>
-  </si>
-  <si>
-    <t>Bras &amp; Tanks</t>
-  </si>
-  <si>
-    <t>Pants</t>
-  </si>
-  <si>
-    <t>Shorts</t>
-  </si>
-  <si>
     <t>menuItemTitle2Sub</t>
   </si>
   <si>
@@ -219,9 +126,6 @@
     <t>productType</t>
   </si>
   <si>
-    <t>Tanks</t>
-  </si>
-  <si>
     <t>h</t>
   </si>
   <si>
@@ -231,69 +135,15 @@
     <t>hoverSubItem</t>
   </si>
   <si>
-    <t>Tops</t>
-  </si>
-  <si>
-    <t>Bottoms</t>
-  </si>
-  <si>
-    <t>Bags</t>
-  </si>
-  <si>
-    <t>Fitness Equipment</t>
-  </si>
-  <si>
-    <t>Watches</t>
-  </si>
-  <si>
     <t>hoverSubSubItem</t>
   </si>
   <si>
-    <t>Video Download</t>
-  </si>
-  <si>
     <t>SI_016</t>
   </si>
   <si>
     <t>SI_017</t>
   </si>
   <si>
-    <t>Wool</t>
-  </si>
-  <si>
-    <t>Style</t>
-  </si>
-  <si>
-    <t>Material</t>
-  </si>
-  <si>
-    <t>Full Zip</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Performance Fabric</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Erin Recommends</t>
-  </si>
-  <si>
-    <t>Color</t>
-  </si>
-  <si>
-    <t>Size</t>
-  </si>
-  <si>
-    <t>XL</t>
-  </si>
-  <si>
-    <t>Green</t>
-  </si>
-  <si>
     <t>categoryWomen1</t>
   </si>
   <si>
@@ -318,9 +168,6 @@
     <t>categoryItemMen2</t>
   </si>
   <si>
-    <t>Workout Pants</t>
-  </si>
-  <si>
     <t>searchRowNumber1</t>
   </si>
   <si>
@@ -339,255 +186,9 @@
     <t>searchRowNumber2</t>
   </si>
   <si>
-    <t>ulrPage</t>
-  </si>
-  <si>
-    <t>Test import data for "Polovni automobili" project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BRZA PRETRAGA </t>
-  </si>
-  <si>
-    <t>subHeaderItemII</t>
-  </si>
-  <si>
-    <t>subHeaderItemI</t>
-  </si>
-  <si>
-    <t>subHeaderItemIII</t>
-  </si>
-  <si>
-    <t>subHeaderItemIV</t>
-  </si>
-  <si>
-    <t>subHeaderItemV</t>
-  </si>
-  <si>
-    <t>subHeaderItemVI</t>
-  </si>
-  <si>
-    <t>subHeaderItemVII</t>
-  </si>
-  <si>
-    <t>subHeaderItemVIII</t>
-  </si>
-  <si>
-    <t>subHeaderItemIX</t>
-  </si>
-  <si>
-    <t>subHeaderItemX</t>
-  </si>
-  <si>
-    <t>subHeaderItemXI</t>
-  </si>
-  <si>
-    <t>Najnoviji oglasi</t>
-  </si>
-  <si>
-    <t>Novi automobili</t>
-  </si>
-  <si>
-    <t>Prvi vlasnik</t>
-  </si>
-  <si>
-    <t>Kupljen nov u Srbiji</t>
-  </si>
-  <si>
-    <t>Automobili na kredit</t>
-  </si>
-  <si>
-    <t>Automobili sa garancijom</t>
-  </si>
-  <si>
-    <t>Pretraga auto usluga</t>
-  </si>
-  <si>
-    <t>Automobili za zamenu</t>
-  </si>
-  <si>
-    <t>Online prodavnica</t>
-  </si>
-  <si>
-    <t>headerItemIb</t>
-  </si>
-  <si>
-    <t>BRZA PRETRAGA</t>
-  </si>
-  <si>
-    <t>headerItemIa</t>
-  </si>
-  <si>
-    <t>Pretraga autoplaceva i kuća</t>
-  </si>
-  <si>
-    <t>Najtraženiji modeli automobila</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PONUDA VOZILA </t>
-  </si>
-  <si>
-    <t>PONUDA VOZILA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DELOVI I OPREMA </t>
-  </si>
-  <si>
-    <t>DELOVI I OPREMA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRODAJEM </t>
-  </si>
-  <si>
-    <t>PRODAJEM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUTO OSIGURANJE </t>
-  </si>
-  <si>
-    <t>AUTO OSIGURANJE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAVETI I VESTI </t>
-  </si>
-  <si>
-    <t>SAVETI I VESTI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USLUGE I KREDITI </t>
-  </si>
-  <si>
-    <t>USLUGE I KREDITI</t>
-  </si>
-  <si>
-    <t>PONUDA ZA OGLAšAVANJE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PONUDA ZA OGLAšAVANJE </t>
-  </si>
-  <si>
-    <t>FIRST</t>
-  </si>
-  <si>
-    <t>SECOND</t>
-  </si>
-  <si>
-    <t>numMenuItem</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Plovila</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Radne mašine</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Motori</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Transportna vozila</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Poljoprivredne mašine</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bicikli</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Putnička vozila</t>
-  </si>
-  <si>
-    <t>subHeaderItemIa</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'Motori</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Karoserija, šasija, limarija</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Elektrika i elektronika</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Motor i mehanički delovi</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Oslanjanje i upravljanje</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Enterijer</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Transmisija</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Izduvni sistem</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Klima, grejanje i ventilacija</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Kočioni sistemi</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Svetla i signalizacija</t>
-  </si>
-  <si>
-    <t>THIRD1</t>
-  </si>
-  <si>
-    <t>THIRD2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Auto oprema</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gume za automobile</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Felne i ratkapne</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Alati za servise</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Kompletan auto u delovima</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Delovi za traktore</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Delovi i oprema za motore</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Delovi i oprema za kamione preko 7,5 tona </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Delovi i oprema za kombije </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gume za traktore</t>
-  </si>
-  <si>
     <t>SI_018</t>
   </si>
   <si>
-    <t xml:space="preserve"> Najnoviji oglasi</t>
-  </si>
-  <si>
-    <t>FORTH</t>
-  </si>
-  <si>
-    <t>Postavi oglas</t>
-  </si>
-  <si>
-    <t>Prodaj sopstveno vozilo</t>
-  </si>
-  <si>
-    <t>Oglasi celokupnu ponudu</t>
-  </si>
-  <si>
-    <t>Ubrzaj prodaju</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
@@ -633,15 +234,6 @@
     <t>najnovijiOglasi</t>
   </si>
   <si>
-    <t>Automobili</t>
-  </si>
-  <si>
-    <t>Asia Motors</t>
-  </si>
-  <si>
-    <t>BMW</t>
-  </si>
-  <si>
     <t>subItem1</t>
   </si>
   <si>
@@ -675,67 +267,88 @@
     <t>subItem10b</t>
   </si>
   <si>
-    <t>Prijavi se</t>
-  </si>
-  <si>
     <t>stjepanovic11temp@gmail.com</t>
   </si>
   <si>
-    <t>stjepatemp</t>
-  </si>
-  <si>
     <t>verificationType</t>
   </si>
   <si>
-    <t>goodCredentials</t>
-  </si>
-  <si>
-    <t>wrongEmail</t>
-  </si>
-  <si>
     <t>rightEmailEnteredYesNo</t>
   </si>
   <si>
-    <t>xxyyyxxxyyy</t>
-  </si>
-  <si>
-    <t>wrongPassword</t>
-  </si>
-  <si>
     <t>verificationText</t>
   </si>
   <si>
-    <t>Ne postoji nalog sa ovom mail adresom.</t>
-  </si>
-  <si>
-    <t>Proveri da li si dobro uneo e-mail i/ili šifru.</t>
-  </si>
-  <si>
-    <t>xxxxyyyxx</t>
-  </si>
-  <si>
-    <t>Krediti</t>
-  </si>
-  <si>
     <t>randomEmailYesNo</t>
   </si>
   <si>
     <t>secondPassword</t>
   </si>
   <si>
-    <t>Mosorinska92</t>
-  </si>
-  <si>
     <t>buttonColor</t>
   </si>
   <si>
-    <t>background-color</t>
-  </si>
-  <si>
-    <t>rgba(255, 165, 0, 1)</t>
-  </si>
-  <si>
     <t>cssType</t>
+  </si>
+  <si>
+    <t>Test import data for "Internet prodaja guma" project</t>
+  </si>
+  <si>
+    <t>gumepasword</t>
+  </si>
+  <si>
+    <t>expectedMessage</t>
+  </si>
+  <si>
+    <t>validEmailPassword</t>
+  </si>
+  <si>
+    <t>emptyEmail</t>
+  </si>
+  <si>
+    <t>emptyPassword</t>
+  </si>
+  <si>
+    <t>emptyEmailPassword</t>
+  </si>
+  <si>
+    <t>InvalidEmailPassword</t>
+  </si>
+  <si>
+    <t>PETAR KOCIC</t>
+  </si>
+  <si>
+    <t>hjeueyue</t>
+  </si>
+  <si>
+    <t>shsjhsjkh@yah.com</t>
+  </si>
+  <si>
+    <t>Polje email je obavezno.</t>
+  </si>
+  <si>
+    <t>Polje password je obavezno.</t>
+  </si>
+  <si>
+    <t>Podaci ne odgovaraju ni jednom nalogu.</t>
+  </si>
+  <si>
+    <t>emptyEmailPasswordMessage2</t>
+  </si>
+  <si>
+    <t>profileSubItem</t>
+  </si>
+  <si>
+    <t>Odjavi se</t>
+  </si>
+  <si>
+    <t>Profil</t>
+  </si>
+  <si>
+    <t>auth/login</t>
+  </si>
+  <si>
+    <t>urlAddressExtension</t>
   </si>
 </sst>
 </file>
@@ -1294,7 +907,7 @@
   <dimension ref="A1:W18"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1326,7 +939,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -1360,49 +973,49 @@
         <v>0</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>185</v>
+        <v>52</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>186</v>
+        <v>53</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>187</v>
+        <v>54</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>188</v>
+        <v>55</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>189</v>
+        <v>56</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>190</v>
+        <v>57</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>191</v>
+        <v>58</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>192</v>
+        <v>59</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>193</v>
+        <v>60</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>194</v>
+        <v>61</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>195</v>
+        <v>62</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>196</v>
+        <v>63</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>197</v>
+        <v>64</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>198</v>
+        <v>65</v>
       </c>
       <c r="P3" s="16" t="s">
-        <v>199</v>
+        <v>66</v>
       </c>
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
@@ -1413,14 +1026,10 @@
     </row>
     <row r="4" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>201</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
@@ -1443,12 +1052,10 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="10"/>
-      <c r="C5" s="11" t="s">
-        <v>202</v>
-      </c>
+      <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
@@ -1471,7 +1078,7 @@
     </row>
     <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="11"/>
@@ -1497,7 +1104,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
@@ -1523,7 +1130,7 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
@@ -1549,7 +1156,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
@@ -1575,7 +1182,7 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
@@ -1601,7 +1208,7 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
@@ -1627,7 +1234,7 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
@@ -1653,7 +1260,7 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
@@ -1679,7 +1286,7 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="11"/>
@@ -1705,7 +1312,7 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="11"/>
@@ -1731,7 +1338,7 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="11"/>
@@ -1757,7 +1364,7 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
@@ -1783,7 +1390,7 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="11"/>
@@ -1824,7 +1431,7 @@
   <dimension ref="A1:AM20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AL12" sqref="AL12"/>
+      <selection sqref="A1:AL1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1867,7 +1474,7 @@
   <sheetData>
     <row r="1" spans="1:38" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -1916,120 +1523,120 @@
         <v>0</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>203</v>
+        <v>67</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>204</v>
+        <v>68</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>205</v>
+        <v>69</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>206</v>
+        <v>70</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>207</v>
+        <v>71</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>208</v>
+        <v>72</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>209</v>
+        <v>73</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>210</v>
+        <v>74</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>211</v>
+        <v>75</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>212</v>
+        <v>76</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>213</v>
+        <v>77</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="U3" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="W3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="X3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF3" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="AK3" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL3" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="S3" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="T3" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="U3" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="V3" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="W3" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="X3" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y3" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z3" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="AA3" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB3" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="AC3" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="AD3" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="AE3" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="AF3" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="AG3" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="AH3" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="AI3" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="AJ3" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AK3" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="AL3" s="7" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="11"/>
@@ -2040,27 +1647,15 @@
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
-      <c r="K4" s="11" t="s">
-        <v>214</v>
-      </c>
+      <c r="K4" s="11"/>
       <c r="L4" s="11"/>
-      <c r="M4" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>216</v>
-      </c>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
       <c r="O4" s="11"/>
-      <c r="P4" s="11" t="s">
-        <v>11</v>
-      </c>
+      <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
-      <c r="R4" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="S4" s="11" t="s">
-        <v>215</v>
-      </c>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
       <c r="T4" s="11"/>
       <c r="U4" s="11"/>
       <c r="V4" s="11"/>
@@ -2081,9 +1676,9 @@
       <c r="AK4" s="11"/>
       <c r="AL4" s="11"/>
     </row>
-    <row r="5" spans="1:38" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
@@ -2094,23 +1689,15 @@
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
-      <c r="K5" s="11" t="s">
-        <v>227</v>
-      </c>
+      <c r="K5" s="11"/>
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
       <c r="O5" s="15"/>
-      <c r="P5" s="15" t="s">
-        <v>13</v>
-      </c>
+      <c r="P5" s="15"/>
       <c r="Q5" s="15"/>
-      <c r="R5" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="S5" s="15" t="s">
-        <v>224</v>
-      </c>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
       <c r="T5" s="15"/>
       <c r="U5" s="11"/>
       <c r="V5" s="11"/>
@@ -2133,7 +1720,7 @@
     </row>
     <row r="6" spans="1:38" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="11"/>
@@ -2146,21 +1733,13 @@
       <c r="J6" s="11"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
-      <c r="M6" s="13" t="s">
-        <v>221</v>
-      </c>
+      <c r="M6" s="13"/>
       <c r="N6" s="11"/>
       <c r="O6" s="15"/>
-      <c r="P6" s="15" t="s">
-        <v>13</v>
-      </c>
+      <c r="P6" s="15"/>
       <c r="Q6" s="15"/>
-      <c r="R6" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="S6" s="15" t="s">
-        <v>224</v>
-      </c>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
       <c r="T6" s="15"/>
       <c r="U6" s="11"/>
       <c r="V6" s="11"/>
@@ -2181,9 +1760,9 @@
       <c r="AK6" s="11"/>
       <c r="AL6" s="11"/>
     </row>
-    <row r="7" spans="1:38" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
@@ -2196,21 +1775,13 @@
       <c r="J7" s="11"/>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
-      <c r="M7" s="11" t="s">
-        <v>215</v>
-      </c>
+      <c r="M7" s="11"/>
       <c r="N7" s="11"/>
       <c r="O7" s="15"/>
-      <c r="P7" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="P7" s="15"/>
       <c r="Q7" s="15"/>
-      <c r="R7" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="S7" s="15" t="s">
-        <v>225</v>
-      </c>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
       <c r="T7" s="15"/>
       <c r="U7" s="11"/>
       <c r="V7" s="11"/>
@@ -2231,9 +1802,9 @@
       <c r="AK7" s="11"/>
       <c r="AL7" s="11"/>
     </row>
-    <row r="8" spans="1:38" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
@@ -2246,23 +1817,13 @@
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
-      <c r="M8" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="N8" s="15" t="s">
-        <v>226</v>
-      </c>
+      <c r="M8" s="11"/>
+      <c r="N8" s="15"/>
       <c r="O8" s="15"/>
-      <c r="P8" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="P8" s="15"/>
       <c r="Q8" s="15"/>
-      <c r="R8" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="S8" s="15" t="s">
-        <v>225</v>
-      </c>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
       <c r="T8" s="15"/>
       <c r="U8" s="11"/>
       <c r="V8" s="15"/>
@@ -2285,7 +1846,7 @@
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
@@ -2299,23 +1860,13 @@
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
-      <c r="N9" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="O9" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="P9" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q9" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
       <c r="R9" s="15"/>
       <c r="S9" s="15"/>
-      <c r="T9" s="15" t="s">
-        <v>233</v>
-      </c>
+      <c r="T9" s="15"/>
       <c r="U9" s="11"/>
       <c r="V9" s="11"/>
       <c r="W9" s="15"/>
@@ -2332,14 +1883,12 @@
       <c r="AH9" s="15"/>
       <c r="AI9" s="15"/>
       <c r="AJ9" s="11"/>
-      <c r="AK9" s="11" t="s">
-        <v>232</v>
-      </c>
+      <c r="AK9" s="11"/>
       <c r="AL9" s="11"/>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
@@ -2381,7 +1930,7 @@
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
@@ -2423,7 +1972,7 @@
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
@@ -2465,7 +2014,7 @@
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
@@ -2507,7 +2056,7 @@
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="11"/>
@@ -2549,7 +2098,7 @@
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="11"/>
@@ -2591,7 +2140,7 @@
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="11"/>
@@ -2633,7 +2182,7 @@
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
@@ -2675,7 +2224,7 @@
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -2718,7 +2267,7 @@
     </row>
     <row r="19" spans="1:39" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>73</v>
+        <v>35</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
@@ -2760,7 +2309,7 @@
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="11"/>
@@ -2815,7 +2364,7 @@
   <dimension ref="A1:W20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2844,7 +2393,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
-        <v>1</v>
+        <v>86</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
@@ -2876,503 +2425,265 @@
         <v>0</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="G3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q3" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="L3" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>92</v>
-      </c>
       <c r="R3" s="8" t="s">
-        <v>93</v>
+        <v>43</v>
       </c>
       <c r="S3" s="8" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="U3" s="8" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="V3" s="8" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="O4" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="P4" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q4" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="R4" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="S4" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="T4" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="U4" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="V4" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>20</v>
-      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
-      <c r="H5" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="J5" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="O5" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="P5" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q5" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="R5" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="S5" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="T5" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="U5" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="V5" s="11" t="s">
-        <v>13</v>
-      </c>
+      <c r="H5" s="11"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11"/>
     </row>
     <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>13</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
-      <c r="E6" s="13" t="s">
-        <v>20</v>
-      </c>
+      <c r="E6" s="13"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
-      <c r="H6" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="L6" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="M6" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="N6" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="O6" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="P6" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q6" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="R6" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="S6" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="T6" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="U6" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="V6" s="11" t="s">
-        <v>13</v>
-      </c>
+      <c r="H6" s="11"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>13</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
-      <c r="E7" s="13" t="s">
-        <v>20</v>
-      </c>
+      <c r="E7" s="13"/>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
-      <c r="H7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>44</v>
-      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="11"/>
       <c r="M7" s="11"/>
-      <c r="N7" s="11" t="s">
-        <v>55</v>
-      </c>
+      <c r="N7" s="11"/>
       <c r="O7" s="11"/>
-      <c r="P7" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q7" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="R7" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="S7" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="T7" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U7" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="V7" s="11" t="s">
-        <v>13</v>
-      </c>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>13</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
-      <c r="E8" s="15" t="s">
-        <v>20</v>
-      </c>
+      <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
-      <c r="H8" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="L8" s="11" t="s">
-        <v>44</v>
-      </c>
+      <c r="H8" s="15"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="11"/>
       <c r="M8" s="15"/>
-      <c r="N8" s="11" t="s">
-        <v>62</v>
-      </c>
+      <c r="N8" s="11"/>
       <c r="O8" s="15"/>
-      <c r="P8" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q8" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="R8" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="S8" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="T8" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="U8" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="V8" s="11" t="s">
-        <v>13</v>
-      </c>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>13</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
-      <c r="E9" s="13" t="s">
-        <v>20</v>
-      </c>
+      <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
-      <c r="H9" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="J9" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="K9" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="L9" s="11" t="s">
-        <v>44</v>
-      </c>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="11"/>
       <c r="M9" s="11"/>
-      <c r="N9" s="15" t="s">
-        <v>57</v>
-      </c>
+      <c r="N9" s="15"/>
       <c r="O9" s="11"/>
-      <c r="P9" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q9" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="R9" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="S9" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="T9" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="U9" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="V9" s="11" t="s">
-        <v>13</v>
-      </c>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="11"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>13</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B10" s="11"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="15" t="s">
-        <v>20</v>
-      </c>
+      <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
-      <c r="H10" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="K10" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="L10" s="11" t="s">
-        <v>44</v>
-      </c>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="11"/>
       <c r="M10" s="6"/>
-      <c r="N10" s="11" t="s">
-        <v>58</v>
-      </c>
+      <c r="N10" s="11"/>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
       <c r="S10" s="6"/>
-      <c r="T10" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="U10" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="V10" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>25</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
-      <c r="H11" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="J11" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="K11" s="15" t="s">
-        <v>69</v>
-      </c>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
@@ -3381,42 +2692,24 @@
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
       <c r="S11" s="6"/>
-      <c r="T11" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="U11" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="V11" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>13</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B12" s="11"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="15" t="s">
-        <v>32</v>
-      </c>
+      <c r="E12" s="15"/>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
-      <c r="H12" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="I12" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="J12" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="K12" s="15" t="s">
-        <v>55</v>
-      </c>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
@@ -3425,42 +2718,24 @@
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
-      <c r="T12" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="U12" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="V12" s="11" t="s">
-        <v>13</v>
-      </c>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="11"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>13</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B13" s="11"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="15" t="s">
-        <v>33</v>
-      </c>
+      <c r="E13" s="15"/>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
-      <c r="H13" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="J13" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="K13" s="15" t="s">
-        <v>72</v>
-      </c>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
@@ -3469,42 +2744,24 @@
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
       <c r="S13" s="6"/>
-      <c r="T13" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U13" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="V13" s="11" t="s">
-        <v>13</v>
-      </c>
+      <c r="T13" s="11"/>
+      <c r="U13" s="11"/>
+      <c r="V13" s="11"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>13</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B14" s="11"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
-      <c r="E14" s="15" t="s">
-        <v>36</v>
-      </c>
+      <c r="E14" s="15"/>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
-      <c r="H14" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="J14" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="K14" s="15" t="s">
-        <v>57</v>
-      </c>
+      <c r="H14" s="15"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
@@ -3513,42 +2770,24 @@
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
       <c r="S14" s="6"/>
-      <c r="T14" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="U14" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="V14" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B15" s="11"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="15" t="s">
-        <v>34</v>
-      </c>
+      <c r="E15" s="15"/>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
-      <c r="H15" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="J15" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="K15" s="15" t="s">
-        <v>57</v>
-      </c>
+      <c r="H15" s="15"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
@@ -3557,42 +2796,24 @@
       <c r="Q15" s="19"/>
       <c r="R15" s="19"/>
       <c r="S15" s="19"/>
-      <c r="T15" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="U15" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="V15" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="T15" s="15"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>13</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B16" s="11"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="15" t="s">
-        <v>37</v>
-      </c>
+      <c r="E16" s="15"/>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
-      <c r="H16" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="I16" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="J16" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="K16" s="15" t="s">
-        <v>70</v>
-      </c>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
@@ -3601,48 +2822,24 @@
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
       <c r="S16" s="6"/>
-      <c r="T16" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="U16" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="V16" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" ht="45.75" x14ac:dyDescent="0.25">
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+      <c r="V16" s="11"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>41</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
       <c r="G17" s="11"/>
-      <c r="H17" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I17" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="J17" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="K17" s="15" t="s">
-        <v>62</v>
-      </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
@@ -3653,13 +2850,11 @@
       <c r="S17" s="6"/>
       <c r="T17" s="6"/>
       <c r="U17" s="6"/>
-      <c r="V17" s="11" t="s">
-        <v>13</v>
-      </c>
+      <c r="V17" s="11"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -3668,15 +2863,9 @@
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
-      <c r="I18" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="J18" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="K18" s="15" t="s">
-        <v>58</v>
-      </c>
+      <c r="I18" s="11"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
@@ -3687,93 +2876,49 @@
       <c r="S18" s="6"/>
       <c r="T18" s="6"/>
       <c r="U18" s="6"/>
-      <c r="V18" s="11" t="s">
-        <v>13</v>
-      </c>
+      <c r="V18" s="11"/>
       <c r="W18" s="6"/>
     </row>
     <row r="19" spans="1:23" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>20</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
       <c r="F19" s="11"/>
-      <c r="G19" s="11" t="s">
-        <v>43</v>
-      </c>
+      <c r="G19" s="11"/>
       <c r="H19" s="11"/>
-      <c r="I19" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="J19" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="K19" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="L19" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="M19" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="N19" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="O19" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
       <c r="P19" s="11"/>
       <c r="Q19" s="11"/>
       <c r="R19" s="11"/>
       <c r="S19" s="11"/>
-      <c r="T19" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="U19" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="V19" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+      <c r="V19" s="11"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>13</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B20" s="11"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="15" t="s">
-        <v>34</v>
-      </c>
+      <c r="E20" s="15"/>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
-      <c r="H20" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="I20" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="J20" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="K20" s="15" t="s">
-        <v>58</v>
-      </c>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
@@ -3782,15 +2927,9 @@
       <c r="Q20" s="19"/>
       <c r="R20" s="19"/>
       <c r="S20" s="19"/>
-      <c r="T20" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="U20" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="V20" s="11" t="s">
-        <v>13</v>
-      </c>
+      <c r="T20" s="15"/>
+      <c r="U20" s="11"/>
+      <c r="V20" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3806,17 +2945,19 @@
   <dimension ref="A1:AH21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
-    <col min="2" max="3" width="14.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="15.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="30" style="1" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="17.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="21" style="1" customWidth="1"/>
     <col min="11" max="11" width="24" style="1" customWidth="1"/>
@@ -3843,7 +2984,7 @@
   <sheetData>
     <row r="1" spans="1:34" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
@@ -3887,56 +3028,36 @@
         <v>0</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>102</v>
+        <v>12</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>146</v>
+        <v>79</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>127</v>
+        <v>88</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="I3" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="J3" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="P3" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q3" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="R3" s="9" t="s">
-        <v>115</v>
-      </c>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
       <c r="S3" s="9"/>
       <c r="T3" s="9"/>
       <c r="U3" s="9"/>
@@ -3956,57 +3077,37 @@
     </row>
     <row r="4" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>78</v>
+      </c>
       <c r="C4" s="11" t="s">
-        <v>9</v>
+        <v>87</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>144</v>
+        <v>89</v>
       </c>
       <c r="E4" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="H4" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="O4" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="P4" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q4" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="R4" s="11" t="s">
-        <v>124</v>
-      </c>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
       <c r="S4" s="11"/>
       <c r="T4" s="11"/>
       <c r="U4" s="11"/>
@@ -4026,43 +3127,29 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
+      <c r="C5" s="11" t="s">
+        <v>87</v>
+      </c>
       <c r="D5" s="11" t="s">
-        <v>145</v>
+        <v>90</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>131</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="F5" s="11"/>
       <c r="G5" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>152</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
       <c r="O5" s="11"/>
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
@@ -4086,50 +3173,30 @@
     </row>
     <row r="6" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="11"/>
+        <v>3</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>78</v>
+      </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11" t="s">
-        <v>166</v>
+        <v>91</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>156</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
       <c r="H6" s="11"/>
-      <c r="I6" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="L6" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="M6" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="N6" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="O6" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="P6" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q6" s="11" t="s">
-        <v>165</v>
-      </c>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
       <c r="R6" s="11"/>
       <c r="S6" s="11"/>
       <c r="T6" s="11"/>
@@ -4150,50 +3217,30 @@
     </row>
     <row r="7" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11" t="s">
-        <v>167</v>
+        <v>92</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>132</v>
+        <v>97</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>168</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="G7" s="11"/>
       <c r="H7" s="11"/>
-      <c r="I7" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="M7" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="N7" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="O7" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="P7" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="Q7" s="11" t="s">
-        <v>177</v>
-      </c>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
       <c r="S7" s="11"/>
       <c r="T7" s="11"/>
@@ -4214,34 +3261,26 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>95</v>
+      </c>
       <c r="D8" s="11" t="s">
-        <v>180</v>
+        <v>93</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>184</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
       <c r="N8" s="6"/>
@@ -4268,17 +3307,21 @@
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>93</v>
+      </c>
       <c r="E9" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>137</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
@@ -4310,17 +3353,21 @@
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+        <v>10</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>93</v>
+      </c>
       <c r="E10" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>139</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="F10" s="11"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
@@ -4352,17 +3399,13 @@
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
-      <c r="E11" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>141</v>
-      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
@@ -4392,19 +3435,15 @@
       <c r="AG11" s="11"/>
       <c r="AH11" s="11"/>
     </row>
-    <row r="12" spans="1:34" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
-      <c r="E12" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>142</v>
-      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
@@ -4436,7 +3475,7 @@
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -4474,7 +3513,7 @@
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -4512,7 +3551,7 @@
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -4550,7 +3589,7 @@
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -4588,7 +3627,7 @@
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -4626,7 +3665,7 @@
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -4664,7 +3703,7 @@
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>73</v>
+        <v>35</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -4702,7 +3741,7 @@
     </row>
     <row r="20" spans="1:34" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -4740,7 +3779,7 @@
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>178</v>
+        <v>51</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>

</xml_diff>

<commit_message>
.gitignore file and  take screenshot method are added
</commit_message>
<xml_diff>
--- a/src/test/test_data/prodajaguma.xlsx
+++ b/src/test/test_data/prodajaguma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QAprojekti\Automation_projekti\Internet_ProdajaGuma\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9544FC-2327-4F9D-A115-6E081818FB7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D352FF-8681-4477-8B4E-5DCA313CD71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="204">
   <si>
     <t>tc_id</t>
   </si>
@@ -620,6 +620,31 @@
   </si>
   <si>
     <t>T (190 KM/H)</t>
+  </si>
+  <si>
+    <t>numberOfTires</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>A6(max 30 km/h)</t>
+  </si>
+  <si>
+    <t>numItems</t>
+  </si>
+  <si>
+    <t>A6(MAX 30 KM/H)</t>
+  </si>
+  <si>
+    <t>Pokušavate da poručite više nego što ima na lageru.
+Maksimalan broj guma koje želite da poručite je</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>205-70-15</t>
   </si>
 </sst>
 </file>
@@ -831,6 +856,9 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -859,9 +887,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1181,7 +1206,7 @@
   <dimension ref="A1:AE29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,53 +1236,54 @@
     <col min="23" max="25" width="14.85546875" style="1" customWidth="1"/>
     <col min="26" max="26" width="53.28515625" style="1" customWidth="1"/>
     <col min="27" max="27" width="15.5703125" style="1" customWidth="1"/>
-    <col min="28" max="29" width="19.140625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="19.140625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="24.5703125" style="1" customWidth="1"/>
     <col min="30" max="30" width="15.5703125" style="1" customWidth="1"/>
     <col min="31" max="31" width="15.28515625" style="1" customWidth="1"/>
     <col min="32" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
     </row>
     <row r="2" spans="1:31" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
     </row>
     <row r="3" spans="1:31" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -1338,10 +1364,18 @@
       <c r="Z3" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="AA3" s="5"/>
-      <c r="AB3" s="5"/>
-      <c r="AC3" s="5"/>
-      <c r="AD3" s="5"/>
+      <c r="AA3" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="AB3" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="AC3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD3" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -1393,11 +1427,14 @@
       <c r="W4" s="11"/>
       <c r="X4" s="11"/>
       <c r="Y4" s="11"/>
-      <c r="Z4" s="11"/>
       <c r="AA4" s="11"/>
       <c r="AB4" s="11"/>
-      <c r="AC4" s="11"/>
-      <c r="AD4" s="11"/>
+      <c r="AC4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD4" s="11" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -1429,7 +1466,7 @@
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
       <c r="O5" s="3" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="P5" s="11" t="s">
         <v>160</v>
@@ -1457,7 +1494,7 @@
       <c r="AC5" s="11"/>
       <c r="AD5" s="11"/>
     </row>
-    <row r="6" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -1480,7 +1517,9 @@
         <v>164</v>
       </c>
       <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
+      <c r="I6" s="11" t="s">
+        <v>159</v>
+      </c>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
@@ -1504,16 +1543,26 @@
       <c r="T6" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="U6" s="11"/>
+      <c r="U6" s="11" t="s">
+        <v>159</v>
+      </c>
       <c r="V6" s="11"/>
       <c r="W6" s="11"/>
       <c r="X6" s="11"/>
       <c r="Y6" s="11"/>
-      <c r="Z6" s="11"/>
+      <c r="Z6" s="11" t="s">
+        <v>201</v>
+      </c>
       <c r="AA6" s="11"/>
-      <c r="AB6" s="11"/>
-      <c r="AC6" s="11"/>
-      <c r="AD6" s="11"/>
+      <c r="AB6" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="AC6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD6" s="11" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1684,7 +1733,9 @@
       <c r="X9" s="11"/>
       <c r="Y9" s="11"/>
       <c r="Z9" s="11"/>
-      <c r="AA9" s="11"/>
+      <c r="AA9" s="11" t="s">
+        <v>197</v>
+      </c>
       <c r="AB9" s="11"/>
       <c r="AC9" s="11"/>
       <c r="AD9" s="11"/>
@@ -1856,8 +1907,12 @@
       <c r="X12" s="11"/>
       <c r="Y12" s="11"/>
       <c r="Z12" s="11"/>
-      <c r="AA12" s="11"/>
-      <c r="AB12" s="11"/>
+      <c r="AA12" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="AB12" s="11" t="s">
+        <v>197</v>
+      </c>
       <c r="AC12" s="11"/>
       <c r="AD12" s="11"/>
     </row>
@@ -1991,7 +2046,9 @@
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
+      <c r="L15" s="11" t="s">
+        <v>198</v>
+      </c>
       <c r="M15" s="11"/>
       <c r="N15" s="11"/>
       <c r="O15" s="3" t="s">
@@ -2009,7 +2066,9 @@
       <c r="S15" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="T15" s="11"/>
+      <c r="T15" s="11" t="s">
+        <v>200</v>
+      </c>
       <c r="U15" s="11"/>
       <c r="V15" s="11"/>
       <c r="W15" s="11"/>
@@ -2176,7 +2235,7 @@
       <c r="C19" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D19" s="32"/>
+      <c r="D19" s="22"/>
       <c r="E19" s="10" t="s">
         <v>153</v>
       </c>
@@ -2191,7 +2250,9 @@
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
+      <c r="O19" s="3" t="s">
+        <v>129</v>
+      </c>
       <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
       <c r="R19" s="6"/>
@@ -2220,7 +2281,7 @@
       <c r="C20" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D20" s="32"/>
+      <c r="D20" s="22"/>
       <c r="E20" s="10" t="s">
         <v>107</v>
       </c>
@@ -2264,7 +2325,7 @@
       <c r="C21" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D21" s="32"/>
+      <c r="D21" s="22"/>
       <c r="E21" s="10" t="s">
         <v>107</v>
       </c>
@@ -2382,35 +2443,59 @@
         <v>94</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D23" s="32"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
-      <c r="R23" s="6"/>
-      <c r="S23" s="6"/>
-      <c r="T23" s="6"/>
-      <c r="U23" s="6"/>
-      <c r="V23" s="6"/>
-      <c r="W23" s="6"/>
-      <c r="X23" s="6"/>
-      <c r="Y23" s="6"/>
-      <c r="Z23" s="6"/>
-      <c r="AA23" s="6"/>
-      <c r="AB23" s="6"/>
-      <c r="AC23" s="6"/>
-      <c r="AD23" s="6"/>
+        <v>120</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="P23" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q23" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="R23" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="S23" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="T23" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="U23" s="11"/>
+      <c r="V23" s="11"/>
+      <c r="W23" s="11"/>
+      <c r="X23" s="11"/>
+      <c r="Y23" s="11"/>
+      <c r="Z23" s="11"/>
+      <c r="AA23" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="AB23" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="AC23" s="11"/>
+      <c r="AD23" s="11"/>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
@@ -2422,7 +2507,7 @@
       <c r="C24" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D24" s="32"/>
+      <c r="D24" s="22"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
@@ -2460,7 +2545,7 @@
       <c r="C25" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D25" s="32"/>
+      <c r="D25" s="22"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
@@ -2498,7 +2583,7 @@
       <c r="C26" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D26" s="32"/>
+      <c r="D26" s="22"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
@@ -2536,7 +2621,7 @@
       <c r="C27" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D27" s="32"/>
+      <c r="D27" s="22"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
@@ -2574,7 +2659,7 @@
       <c r="C28" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D28" s="32"/>
+      <c r="D28" s="22"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
@@ -2612,7 +2697,7 @@
       <c r="C29" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D29" s="32"/>
+      <c r="D29" s="22"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
@@ -2758,55 +2843,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="27"/>
-      <c r="AL1" s="27"/>
-      <c r="AM1" s="27"/>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="27"/>
-      <c r="AP1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="28"/>
+      <c r="AG1" s="28"/>
+      <c r="AH1" s="28"/>
+      <c r="AI1" s="28"/>
+      <c r="AJ1" s="28"/>
+      <c r="AK1" s="28"/>
+      <c r="AL1" s="28"/>
+      <c r="AM1" s="28"/>
+      <c r="AN1" s="28"/>
+      <c r="AO1" s="28"/>
+      <c r="AP1" s="28"/>
     </row>
     <row r="2" spans="1:42" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
     </row>
     <row r="3" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -3811,41 +3896,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="29"/>
-      <c r="U1" s="29"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="29"/>
-      <c r="AD1" s="29"/>
-      <c r="AE1" s="29"/>
-      <c r="AF1" s="29"/>
-      <c r="AG1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
     </row>
     <row r="2" spans="1:33" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>
@@ -4641,7 +4726,7 @@
   <dimension ref="A1:AH21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4679,42 +4764,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
     </row>
     <row r="2" spans="1:34" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>

</xml_diff>

<commit_message>
Dev and master branch are merged
</commit_message>
<xml_diff>
--- a/src/test/test_data/prodajaguma.xlsx
+++ b/src/test/test_data/prodajaguma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QAprojekti\Automation_projekti\Internet_ProdajaGuma\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D352FF-8681-4477-8B4E-5DCA313CD71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0D841B-EBA5-4F2B-AA25-894BCA8084D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="gume" sheetId="1" r:id="rId1"/>
@@ -1205,7 +1205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1AEBA6-E97B-44CC-BE50-33F6B24023CF}">
   <dimension ref="A1:AE29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -4725,8 +4725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D05107-472F-4DD1-88F8-DE97CAF36E00}">
   <dimension ref="A1:AH21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
BasePage class has refactored
</commit_message>
<xml_diff>
--- a/src/test/test_data/prodajaguma.xlsx
+++ b/src/test/test_data/prodajaguma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QAprojekti\Automation_projekti\Internet_ProdajaGuma\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0D841B-EBA5-4F2B-AA25-894BCA8084D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8486BB43-302F-4147-BE95-0F149B18D096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="gume" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="206">
   <si>
     <t>tc_id</t>
   </si>
@@ -645,6 +645,12 @@
   </si>
   <si>
     <t>205-70-15</t>
+  </si>
+  <si>
+    <t>MIN. CENA: 4900</t>
+  </si>
+  <si>
+    <t>MAX. CENA: 35750</t>
   </si>
 </sst>
 </file>
@@ -1205,8 +1211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1AEBA6-E97B-44CC-BE50-33F6B24023CF}">
   <dimension ref="A1:AE29"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,10 +1484,10 @@
         <v>164</v>
       </c>
       <c r="S5" s="11" t="s">
-        <v>162</v>
+        <v>204</v>
       </c>
       <c r="T5" s="11" t="s">
-        <v>163</v>
+        <v>205</v>
       </c>
       <c r="U5" s="11"/>
       <c r="V5" s="11"/>
@@ -1538,10 +1544,10 @@
         <v>164</v>
       </c>
       <c r="S6" s="11" t="s">
-        <v>162</v>
+        <v>204</v>
       </c>
       <c r="T6" s="11" t="s">
-        <v>163</v>
+        <v>205</v>
       </c>
       <c r="U6" s="11" t="s">
         <v>159</v>
@@ -2409,10 +2415,10 @@
         <v>164</v>
       </c>
       <c r="S22" s="11" t="s">
-        <v>162</v>
+        <v>204</v>
       </c>
       <c r="T22" s="11" t="s">
-        <v>163</v>
+        <v>205</v>
       </c>
       <c r="U22" s="11" t="s">
         <v>159</v>
@@ -4725,7 +4731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D05107-472F-4DD1-88F8-DE97CAF36E00}">
   <dimension ref="A1:AH21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>